<commit_message>
Uploading new codes from my studies on Alura
</commit_message>
<xml_diff>
--- a/Alura/Visualizacao/02 - Escolhendo o melhor gráfico/Data visualization 02 - Planilha de gastos.xlsx
+++ b/Alura/Visualizacao/02 - Escolhendo o melhor gráfico/Data visualization 02 - Planilha de gastos.xlsx
@@ -5,6 +5,8 @@
   <sheets>
     <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Página2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Página4" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Página5" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="21">
   <si>
     <t>Faculdade</t>
   </si>
@@ -33,6 +35,9 @@
   </si>
   <si>
     <t>Janeiro</t>
+  </si>
+  <si>
+    <t>Drill down</t>
   </si>
   <si>
     <t>Fevereiro</t>
@@ -67,12 +72,18 @@
   <si>
     <t>Dezembro</t>
   </si>
+  <si>
+    <t>Treino</t>
+  </si>
+  <si>
+    <t>Aluguel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -82,6 +93,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -97,14 +109,25 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -227,11 +250,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="169767339"/>
-        <c:axId val="1622037863"/>
+        <c:axId val="1767467156"/>
+        <c:axId val="2028095042"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169767339"/>
+        <c:axId val="1767467156"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -283,10 +306,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1622037863"/>
+        <c:crossAx val="2028095042"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1622037863"/>
+        <c:axId val="2028095042"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -352,8 +375,800 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169767339"/>
+        <c:crossAx val="1767467156"/>
         <c:crosses val="max"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Faculdade, Transporte, Lazer, Internet, Cartão de crédito…</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$B$17</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$18:$A$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$18:$B$27</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$C$17</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$18:$A$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$C$18:$C$27</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$D$17</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$18:$A$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$D$18:$D$27</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$E$17</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$18:$A$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$E$18:$E$27</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$F$17</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D01"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$18:$A$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$F$18:$F$27</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$G$17</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="46BDC6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$18:$A$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$G$18:$G$27</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1915990235"/>
+        <c:axId val="248548935"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="1915990235"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="248548935"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="248548935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1915990235"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Faculdade, Transporte, Lazer, Internet, Cartão de crédito…</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$A$18</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$B$17:$G$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$18:$G$18</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$A$19</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$B$17:$G$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$19:$G$19</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$A$20</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$B$17:$G$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$20:$G$20</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$A$21</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$B$17:$G$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$21:$G$21</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$A$22</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D01"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$B$17:$G$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$22:$G$22</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$A$23</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="46BDC6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$B$17:$G$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$23:$G$23</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$A$24</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="7BAAF7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$B$17:$G$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$24:$G$24</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="2002518575"/>
+        <c:axId val="532571030"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2002518575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532571030"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="532571030"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2002518575"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -460,11 +1275,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1311690739"/>
-        <c:axId val="1289067062"/>
+        <c:axId val="981426557"/>
+        <c:axId val="512960398"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1311690739"/>
+        <c:axId val="981426557"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -516,10 +1331,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1289067062"/>
+        <c:crossAx val="512960398"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1289067062"/>
+        <c:axId val="512960398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +1400,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1311690739"/>
+        <c:crossAx val="981426557"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -613,6 +1428,811 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$B$2:$B$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$C$2:$C$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$D$2:$D$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$E$2:$E$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$F$2:$F$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$G$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$G$2:$G$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="1125532818"/>
+        <c:axId val="1730606650"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1125532818"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1730606650"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1730606650"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1125532818"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$B$2:$B$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$C$2:$C$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$D$2:$D$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$E$2:$E$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$F$2:$F$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$G$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$G$2:$G$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1333038735"/>
+        <c:axId val="190092333"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1333038735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="190092333"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="190092333"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1333038735"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -839,11 +2459,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="681693718"/>
-        <c:axId val="2123580830"/>
+        <c:axId val="1756347666"/>
+        <c:axId val="871937568"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="681693718"/>
+        <c:axId val="1756347666"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,10 +2515,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123580830"/>
+        <c:crossAx val="871937568"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123580830"/>
+        <c:axId val="871937568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,7 +2593,1998 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="681693718"/>
+        <c:crossAx val="1756347666"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>2017, 2018, 2016, 2015 e 2014</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$B$2:$B$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$C$2:$C$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$D$2:$D$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$E$2:$E$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$F$2:$F$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$G$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$G$2:$G$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$H$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumOff val="30000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$H$2:$H$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$I$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumOff val="30000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$I$2:$I$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="139871030"/>
+        <c:axId val="1330168782"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="139871030"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1330168782"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1330168782"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="139871030"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>2017, 2018, 2016, 2015 e 2014</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$B$2:$B$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$C$2:$C$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$D$2:$D$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$E$2:$E$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$F$2:$F$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$G$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$G$2:$G$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$H$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumOff val="30000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$H$2:$H$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$I$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumOff val="30000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$I$2:$I$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="2022229274"/>
+        <c:axId val="986287931"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2022229274"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="986287931"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="986287931"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2022229274"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Faculdade, Transporte, Lazer, Internet, Cartão de crédito…</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$B$2:$B$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$C$2:$C$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$D$2:$D$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$E$2:$E$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D01"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$F$2:$F$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$G$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="46BDC6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$G$2:$G$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$H$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="7BAAF7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$H$2:$H$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página4'!$I$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="F07B72"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página4'!$A$2:$A$6</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página4'!$I$2:$I$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1755305801"/>
+        <c:axId val="124982922"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="1755305801"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="124982922"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="124982922"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1755305801"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Faculdade, Transporte, Lazer, Internet, Cartão de crédito…</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$2:$A$13</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$B$2:$B$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$2:$A$13</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$C$2:$C$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$2:$A$13</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$D$2:$D$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$2:$A$13</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$E$2:$E$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF6D01"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$2:$A$13</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$F$2:$F$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página5'!$G$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="46BDC6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página5'!$A$2:$A$13</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página5'!$G$2:$G$13</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="961480222"/>
+        <c:axId val="1718234692"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="961480222"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1718234692"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1718234692"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="961480222"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1005,8 +4616,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5514975" cy="3400425"/>
     <xdr:graphicFrame>
@@ -1030,8 +4641,8 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5514975" cy="3400425"/>
     <xdr:graphicFrame>
@@ -1051,19 +4662,14 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6600825" cy="4086225"/>
+    <xdr:ext cx="5514975" cy="3400425"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
@@ -1075,7 +4681,222 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5514975" cy="3400425"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6600825" cy="4086225"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6743700" cy="4171950"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6743700" cy="4171950"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 7" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6305550" cy="3905250"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 8" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 9" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 10" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 11" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1354,32 +5175,6 @@
         <v>1243.0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="2">
-        <f t="shared" ref="B4:G4" si="1">sum(B2,B3)</f>
-        <v>24700</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" si="1"/>
-        <v>10000</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" si="1"/>
-        <v>6396</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="1"/>
-        <v>1205</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="1"/>
-        <v>10547</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="1"/>
-        <v>3172</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1437,10 +5232,13 @@
       <c r="G2" s="1">
         <v>260.0</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>2300.0</v>
@@ -1463,7 +5261,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>2300.0</v>
@@ -1486,7 +5284,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>2300.0</v>
@@ -1509,7 +5307,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>2300.0</v>
@@ -1532,7 +5330,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>2300.0</v>
@@ -1555,7 +5353,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>2000.0</v>
@@ -1578,7 +5376,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>2300.0</v>
@@ -1601,7 +5399,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>2300.0</v>
@@ -1624,7 +5422,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>2300.0</v>
@@ -1647,7 +5445,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>2300.0</v>
@@ -1670,7 +5468,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>2000.0</v>
@@ -1689,6 +5487,685 @@
       </c>
       <c r="G13" s="1">
         <v>170.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>2014.0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4432.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2200.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>520.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2021.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1872.0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>150.0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <v>2015.0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>24400.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4529.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3250.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>540.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1298.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1347.0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>150.0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>2016.0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>24400.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4448.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3000.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>600.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2654.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1821.0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>180.0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>2017.0</v>
+      </c>
+      <c r="B5" s="4">
+        <v>24400.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5540.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4020.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>643.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>7060.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1929.0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>150.0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>2018.0</v>
+      </c>
+      <c r="B6" s="4">
+        <v>300.0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4460.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2376.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>562.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3487.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1243.0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>130.0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>900.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>230.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>260.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>520.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>240.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>550.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>260.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>180.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>480.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>432.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>57.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>460.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>430.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>430.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>335.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>190.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>276.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>160.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>530.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>348.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>69.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>560.0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>180.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>520.0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>564.0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>68.0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>700.0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>189.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>550.0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>53.0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>460.0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>535.0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>170.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2000.0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>500.0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>230.0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>50.0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>900.0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>260.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2300.0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>520.0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>240.0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>60.0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>500.0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>480.0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>432.0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>57.0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="5">
+        <v>2300.0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>460.0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>430.0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>56.0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>600.0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2300.0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>430.0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>335.0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>62.0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>800.0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>190.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2000.0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>500.0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>276.0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>65.0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>900.0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>160.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2300.0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>550.0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>53.0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>100.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>